<commit_message>
summary:     Added Jint benchmark date:        Thu Jul 22 14:54:43 2010 +0000 user:        paulbartrum changeset:   11:2573878cf37a hg2git:      Preserving hg log changeset
</commit_message>
<xml_diff>
--- a/Performance/Sunspider.xlsx
+++ b/Performance/Sunspider.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="390" windowWidth="10275" windowHeight="9240"/>
+    <workbookView xWindow="600" yWindow="390" windowWidth="10275" windowHeight="9240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Historical Times" sheetId="4" r:id="rId1"/>
@@ -248,6 +248,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
   <fonts count="21">
     <font>
       <sz val="11"/>
@@ -802,22 +805,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1155,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1171,262 +1173,267 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="13"/>
+      <c r="A2" s="6"/>
     </row>
     <row r="3" spans="1:2" ht="21" thickBot="1">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="13">
+      <c r="A4" s="6">
         <v>40348</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="7">
         <v>40355</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="13">
+      <c r="A5" s="6">
         <v>40373</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="7">
         <v>25772</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="B6" s="14"/>
+      <c r="A6" s="6">
+        <v>40382</v>
+      </c>
+      <c r="B6" s="7">
+        <v>24471</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="B7" s="14"/>
+      <c r="B7" s="7"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="B8" s="14"/>
+      <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="B9" s="14"/>
+      <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="B10" s="14"/>
+      <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="B11" s="14"/>
+      <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="B12" s="14"/>
+      <c r="B12" s="7"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="B13" s="14"/>
+      <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="B14" s="14"/>
+      <c r="B14" s="7"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="B15" s="14"/>
+      <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="B16" s="14"/>
+      <c r="B16" s="7"/>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="14"/>
+      <c r="B17" s="7"/>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="14"/>
+      <c r="B18" s="7"/>
     </row>
     <row r="19" spans="2:2">
-      <c r="B19" s="14"/>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" s="14"/>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" spans="2:2">
-      <c r="B21" s="14"/>
+      <c r="B21" s="7"/>
     </row>
     <row r="22" spans="2:2">
-      <c r="B22" s="14"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="14"/>
+      <c r="B23" s="7"/>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="14"/>
+      <c r="B24" s="7"/>
     </row>
     <row r="25" spans="2:2">
-      <c r="B25" s="14"/>
+      <c r="B25" s="7"/>
     </row>
     <row r="26" spans="2:2">
-      <c r="B26" s="14"/>
+      <c r="B26" s="7"/>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" s="14"/>
+      <c r="B27" s="7"/>
     </row>
     <row r="28" spans="2:2">
-      <c r="B28" s="14"/>
+      <c r="B28" s="7"/>
     </row>
     <row r="29" spans="2:2">
-      <c r="B29" s="14"/>
+      <c r="B29" s="7"/>
     </row>
     <row r="30" spans="2:2">
-      <c r="B30" s="14"/>
+      <c r="B30" s="7"/>
     </row>
     <row r="31" spans="2:2">
-      <c r="B31" s="14"/>
+      <c r="B31" s="7"/>
     </row>
     <row r="32" spans="2:2">
-      <c r="B32" s="14"/>
+      <c r="B32" s="7"/>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="14"/>
+      <c r="B33" s="7"/>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="14"/>
+      <c r="B34" s="7"/>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="14"/>
+      <c r="B35" s="7"/>
     </row>
     <row r="36" spans="2:2">
-      <c r="B36" s="14"/>
+      <c r="B36" s="7"/>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="14"/>
+      <c r="B37" s="7"/>
     </row>
     <row r="38" spans="2:2">
-      <c r="B38" s="14"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="14"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="14"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="14"/>
+      <c r="B41" s="7"/>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="14"/>
+      <c r="B42" s="7"/>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="14"/>
+      <c r="B43" s="7"/>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="14"/>
+      <c r="B44" s="7"/>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="14"/>
+      <c r="B45" s="7"/>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="14"/>
+      <c r="B46" s="7"/>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="14"/>
+      <c r="B47" s="7"/>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="14"/>
+      <c r="B48" s="7"/>
     </row>
     <row r="49" spans="2:2">
-      <c r="B49" s="14"/>
+      <c r="B49" s="7"/>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" s="14"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" spans="2:2">
-      <c r="B51" s="14"/>
+      <c r="B51" s="7"/>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="14"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" s="14"/>
+      <c r="B53" s="7"/>
     </row>
     <row r="54" spans="2:2">
-      <c r="B54" s="14"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="14"/>
+      <c r="B55" s="7"/>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" s="14"/>
+      <c r="B56" s="7"/>
     </row>
     <row r="57" spans="2:2">
-      <c r="B57" s="14"/>
+      <c r="B57" s="7"/>
     </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="14"/>
+      <c r="B58" s="7"/>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="14"/>
+      <c r="B59" s="7"/>
     </row>
     <row r="60" spans="2:2">
-      <c r="B60" s="14"/>
+      <c r="B60" s="7"/>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="14"/>
+      <c r="B61" s="7"/>
     </row>
     <row r="62" spans="2:2">
-      <c r="B62" s="14"/>
+      <c r="B62" s="7"/>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="14"/>
+      <c r="B63" s="7"/>
     </row>
     <row r="64" spans="2:2">
-      <c r="B64" s="14"/>
+      <c r="B64" s="7"/>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="14"/>
+      <c r="B65" s="7"/>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="14"/>
+      <c r="B66" s="7"/>
     </row>
     <row r="67" spans="2:2">
-      <c r="B67" s="14"/>
+      <c r="B67" s="7"/>
     </row>
     <row r="68" spans="2:2">
-      <c r="B68" s="14"/>
+      <c r="B68" s="7"/>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="14"/>
+      <c r="B69" s="7"/>
     </row>
     <row r="70" spans="2:2">
-      <c r="B70" s="14"/>
+      <c r="B70" s="7"/>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="14"/>
+      <c r="B71" s="7"/>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="14"/>
+      <c r="B72" s="7"/>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="14"/>
+      <c r="B73" s="7"/>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="14"/>
+      <c r="B74" s="7"/>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="14"/>
+      <c r="B75" s="7"/>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="14"/>
+      <c r="B76" s="7"/>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="14"/>
+      <c r="B77" s="7"/>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="14"/>
+      <c r="B78" s="7"/>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="14"/>
+      <c r="B79" s="7"/>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="14"/>
+      <c r="B80" s="7"/>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="14"/>
+      <c r="B81" s="7"/>
     </row>
     <row r="82" spans="2:2">
-      <c r="B82" s="14"/>
+      <c r="B82" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1437,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1460,27 +1467,27 @@
       <c r="A3" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="13">
-        <v>40373</v>
+      <c r="B3" s="6">
+        <v>40382</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21" thickBot="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="5" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1488,546 +1495,547 @@
       <c r="A6" t="s">
         <v>63</v>
       </c>
-      <c r="B6">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>27.3</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>182.7</v>
-      </c>
-      <c r="F6" s="5">
-        <v>224.9</v>
+      <c r="B6" s="8">
+        <v>13.5</v>
+      </c>
+      <c r="C6" s="8">
+        <v>32</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>199.1</v>
+      </c>
+      <c r="F6" s="9">
+        <v>244.5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>62</v>
       </c>
-      <c r="B7">
-        <v>0.6</v>
-      </c>
-      <c r="C7">
-        <v>0.5</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>369.6</v>
+      <c r="B7" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>310.2</v>
       </c>
       <c r="F7" s="10">
-        <v>370.7</v>
+        <v>311.3</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>61</v>
       </c>
-      <c r="B8">
-        <v>7.1</v>
-      </c>
-      <c r="C8">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>465.4</v>
+      <c r="B8" s="8">
+        <v>3.7</v>
+      </c>
+      <c r="C8" s="8">
+        <v>15.8</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>500.3</v>
       </c>
       <c r="F8" s="10">
-        <v>481.8</v>
+        <v>519.79999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
         <v>0.3</v>
       </c>
-      <c r="C9">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D9">
+      <c r="C9" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="8">
         <v>0</v>
       </c>
       <c r="E9" s="8">
-        <v>932.4</v>
-      </c>
-      <c r="F9" s="9">
-        <v>933.8</v>
+        <v>1003.7</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1005.2</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>59</v>
       </c>
-      <c r="B10">
-        <v>0.9</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
+      <c r="B10" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2</v>
+      </c>
+      <c r="D10" s="8">
         <v>0</v>
       </c>
       <c r="E10" s="8">
-        <v>1060.3</v>
-      </c>
-      <c r="F10" s="9">
-        <v>1065.2</v>
+        <v>930.9</v>
+      </c>
+      <c r="F10" s="10">
+        <v>933.5</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>58</v>
       </c>
-      <c r="B11">
-        <v>1.5</v>
-      </c>
-      <c r="C11">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>412.4</v>
+      <c r="B11" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1.9</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>333.8</v>
       </c>
       <c r="F11" s="10">
-        <v>416.3</v>
+        <v>336.9</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>57</v>
       </c>
-      <c r="B12">
-        <v>0.3</v>
-      </c>
-      <c r="C12">
-        <v>0.6</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>367.2</v>
+      <c r="B12" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>322.60000000000002</v>
       </c>
       <c r="F12" s="10">
-        <v>368</v>
+        <v>323.2</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>56</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="8">
         <v>0.2</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="8">
         <v>0.2</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>81.900000000000006</v>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>222.1</v>
       </c>
       <c r="F13" s="10">
-        <v>82.3</v>
+        <v>222.5</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>55</v>
       </c>
-      <c r="B14">
-        <v>0.1</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="8">
         <v>0.4</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>78.8</v>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
+        <v>149.80000000000001</v>
       </c>
       <c r="F14" s="10">
-        <v>79.3</v>
+        <v>150.4</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>54</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="8">
         <v>0.1</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="8">
         <v>0.1</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>499.2</v>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
+        <v>283.5</v>
       </c>
       <c r="F15" s="10">
-        <v>499.4</v>
+        <v>283.60000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>53</v>
       </c>
-      <c r="B16">
-        <v>0.3</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="C16" s="8">
         <v>0.5</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>279</v>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
+        <v>273.89999999999998</v>
       </c>
       <c r="F16" s="10">
-        <v>279.8</v>
+        <v>274.7</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>52</v>
       </c>
-      <c r="B17">
-        <v>0.2</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="C17" s="8">
         <v>0.4</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>54.4</v>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
+        <v>153</v>
       </c>
       <c r="F17" s="10">
-        <v>55</v>
+        <v>153.6</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>51</v>
       </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18">
-        <v>10.5</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>658.1</v>
+      <c r="B18" s="8">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C18" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8">
+        <v>663.6</v>
       </c>
       <c r="F18" s="10">
-        <v>673.7</v>
+        <v>676</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>50</v>
       </c>
-      <c r="B19">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C19">
-        <v>5.8</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>464.4</v>
+      <c r="B19" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="C19" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8">
+        <v>505.1</v>
       </c>
       <c r="F19" s="10">
-        <v>474.3</v>
+        <v>511.7</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>49</v>
       </c>
-      <c r="B20">
-        <v>1.6</v>
-      </c>
-      <c r="C20">
-        <v>3.3</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>323.10000000000002</v>
+      <c r="B20" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
+        <v>313.3</v>
       </c>
       <c r="F20" s="10">
-        <v>328</v>
+        <v>316.7</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>48</v>
       </c>
-      <c r="B21">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C21">
-        <v>2.6</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>477.4</v>
+      <c r="B21" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2.4</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8">
+        <v>427.5</v>
       </c>
       <c r="F21" s="10">
-        <v>482.4</v>
+        <v>431.7</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>47</v>
       </c>
-      <c r="B22">
-        <v>5.3</v>
-      </c>
-      <c r="C22">
-        <v>3.5</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>329.8</v>
+      <c r="B22" s="8">
+        <v>6.1</v>
+      </c>
+      <c r="C22" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8">
+        <v>321.10000000000002</v>
       </c>
       <c r="F22" s="10">
-        <v>338.6</v>
+        <v>330.6</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>46</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="8">
         <v>0.4</v>
       </c>
-      <c r="C23">
-        <v>0.7</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>270.8</v>
+      <c r="C23" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8">
+        <v>317.8</v>
       </c>
       <c r="F23" s="10">
-        <v>271.89999999999998</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="8">
         <v>0.3</v>
       </c>
-      <c r="C24">
-        <v>0.5</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>277.2</v>
+      <c r="C24" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8">
+        <v>181.7</v>
       </c>
       <c r="F24" s="10">
-        <v>277.89999999999998</v>
+        <v>182.6</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>44</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="8">
         <v>0.4</v>
       </c>
-      <c r="C25">
-        <v>0.8</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>172.4</v>
+      <c r="C25" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0</v>
+      </c>
+      <c r="E25" s="8">
+        <v>252.1</v>
       </c>
       <c r="F25" s="10">
-        <v>173.5</v>
+        <v>253.2</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>43</v>
       </c>
-      <c r="B26">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="8">
+        <v>1.6</v>
+      </c>
+      <c r="C26" s="8">
         <v>0.8</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>849.6</v>
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="8">
+        <v>768.4</v>
       </c>
       <c r="F26" s="10">
-        <v>852.7</v>
+        <v>770.8</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>42</v>
       </c>
-      <c r="B27">
-        <v>1.5</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="8">
         <v>1.2</v>
       </c>
-      <c r="D27">
+      <c r="C27" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D27" s="8">
         <v>0</v>
       </c>
       <c r="E27" s="8">
-        <v>1871</v>
-      </c>
-      <c r="F27" s="9">
-        <v>1873.7</v>
+        <v>1222.5999999999999</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1224.8</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>41</v>
       </c>
-      <c r="B28">
-        <v>0.4</v>
-      </c>
-      <c r="C28">
-        <v>0.7</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>599.29999999999995</v>
+      <c r="B28" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0</v>
+      </c>
+      <c r="E28" s="8">
+        <v>484.7</v>
       </c>
       <c r="F28" s="10">
-        <v>600.4</v>
+        <v>486.3</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>40</v>
       </c>
-      <c r="B29">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C29">
-        <v>2.5</v>
-      </c>
-      <c r="D29">
+      <c r="B29" s="8">
+        <v>4</v>
+      </c>
+      <c r="C29" s="8">
+        <v>2.1</v>
+      </c>
+      <c r="D29" s="8">
         <v>0</v>
       </c>
       <c r="E29" s="8">
-        <v>2581</v>
-      </c>
-      <c r="F29" s="9">
-        <v>2587.6</v>
+        <v>3284.7</v>
+      </c>
+      <c r="F29" s="10">
+        <v>3290.8</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>39</v>
       </c>
-      <c r="B30">
-        <v>15.7</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-      <c r="D30">
+      <c r="B30" s="8">
+        <v>16</v>
+      </c>
+      <c r="C30" s="8">
+        <v>3.9</v>
+      </c>
+      <c r="D30" s="8">
         <v>0</v>
       </c>
       <c r="E30" s="8">
-        <v>4066.6</v>
-      </c>
-      <c r="F30" s="9">
-        <v>4085.3</v>
+        <v>3670.4</v>
+      </c>
+      <c r="F30" s="10">
+        <v>3690.4</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1">
       <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="B31">
-        <v>0.6</v>
-      </c>
-      <c r="C31">
-        <v>0.9</v>
-      </c>
-      <c r="D31">
+      <c r="B31" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="D31" s="8">
         <v>0</v>
       </c>
       <c r="E31" s="8">
-        <v>7894.8</v>
-      </c>
-      <c r="F31" s="7">
-        <v>7896.3</v>
+        <v>7226.7</v>
+      </c>
+      <c r="F31" s="11">
+        <v>7228</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="B32" s="6">
+      <c r="B32" s="12">
         <f>SUM(B6:B31)</f>
-        <v>70.499999999999986</v>
-      </c>
-      <c r="C32" s="6">
+        <v>62.8</v>
+      </c>
+      <c r="C32" s="12">
         <f>SUM(C6:C31)</f>
-        <v>83.5</v>
-      </c>
-      <c r="D32" s="6">
+        <v>86.399999999999991</v>
+      </c>
+      <c r="D32" s="12">
         <f>SUM(D6:D31)</f>
         <v>0</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="12">
         <f>SUM(E6:E31)</f>
-        <v>25618.799999999996</v>
-      </c>
-      <c r="F32" s="12">
+        <v>24322.600000000006</v>
+      </c>
+      <c r="F32" s="13">
         <f>SUM(F6:F31)</f>
-        <v>25772.799999999999</v>
+        <v>24471.8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>